<commit_message>
not many shows and venues, but very clean interface/functionality
</commit_message>
<xml_diff>
--- a/zingvenues.xlsx
+++ b/zingvenues.xlsx
@@ -6,12 +6,14 @@
   </bookViews>
   <sheets>
     <sheet name="PhillyVenues" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="128">
   <si>
     <t>name</t>
   </si>
@@ -40,6 +42,9 @@
     <t>twitter</t>
   </si>
   <si>
+    <t>tix</t>
+  </si>
+  <si>
     <t>Arden Theatre Company</t>
   </si>
   <si>
@@ -50,7 +55,7 @@
   </si>
   <si>
     <t>40 N. 2nd Street, 
-Philadelphia, PA 19106</t>
+Philadelphia</t>
   </si>
   <si>
     <t xml:space="preserve">215.922.1122
@@ -69,6 +74,9 @@
     <t>https://twitter.com/ArdenTheatreCo</t>
   </si>
   <si>
+    <t>http://www.ardentheatre.org/tickets/</t>
+  </si>
+  <si>
     <t>Storybook Musical Theatre</t>
   </si>
   <si>
@@ -78,8 +86,7 @@
     <t>Founded in 1992, Storybook Musical Theatre's mission is the cultural enrichment and education of children and their families by introducing them to and developing a life-long appreciation for musical theater through original adaptations of folk tales and children's literature.</t>
   </si>
   <si>
-    <t>P.O. Box 473, 
-Abington, PA 19001</t>
+    <t>1811 Edge Hill Rd, Abington</t>
   </si>
   <si>
     <t xml:space="preserve">215.659.8550
@@ -95,6 +102,9 @@
     <t>https://twitter.com/StorybookMagic</t>
   </si>
   <si>
+    <t>http://www.storybookmusical.org/tickets.html</t>
+  </si>
+  <si>
     <t>Act II Playhouse</t>
   </si>
   <si>
@@ -105,7 +115,7 @@
   </si>
   <si>
     <t>56 E. Butler Avenue, 
-Ambler, PA 19002</t>
+Ambler</t>
   </si>
   <si>
     <t xml:space="preserve">215.654.0200
@@ -124,6 +134,9 @@
     <t>https://twitter.com/act2playhouse</t>
   </si>
   <si>
+    <t>http://act2.org/cms2/index.php/tickets</t>
+  </si>
+  <si>
     <t>The Wilma Theater</t>
   </si>
   <si>
@@ -134,7 +147,7 @@
   </si>
   <si>
     <t>265 S. Broad Street, 
-Philadelphia, PA 19107</t>
+Philadelphia</t>
   </si>
   <si>
     <t xml:space="preserve">215.546.7824
@@ -153,6 +166,9 @@
     <t>https://twitter.com/thewilmatheater</t>
   </si>
   <si>
+    <t>https://www.wilmatheater.org/tickets</t>
+  </si>
+  <si>
     <t>Lantern Theater Company</t>
   </si>
   <si>
@@ -162,8 +178,7 @@
     <t>Lantern Theater Company is committed to an authentic and intimate exploration of the human spirit in our choice of classics, modern, and original works. We reach a loyal, diverse, and growing annual audience of 20,000 through three award-winning programs: Mainstage Productions that are smart, fun, engaging, and connected to our modern world; Lantern Theater Company: In Conversation, our audience engagement series that offers an insider's look at each production with artists and guest scholars; and &lt;i&gt;Illumination&lt;/i&gt;, our innovative education program that engages local students in the world of theater and nurtures their artistic expression.</t>
   </si>
   <si>
-    <t>St. Stephen's Theater, 
-10th &amp; Ludlow Street</t>
+    <t>10th &amp; Ludlow Streets, Philadelphia</t>
   </si>
   <si>
     <t xml:space="preserve">215.829.0395
@@ -182,6 +197,9 @@
     <t>https://twitter.com/lanterntheater</t>
   </si>
   <si>
+    <t>http://www.lanterntheater.org/tickets/</t>
+  </si>
+  <si>
     <t>The Eagle Theatre</t>
   </si>
   <si>
@@ -192,7 +210,7 @@
   </si>
   <si>
     <t>208 Vine Street, 
-Hammonton, NJ 08037</t>
+Hammonton, NJ</t>
   </si>
   <si>
     <t xml:space="preserve">609.704.5012
@@ -211,6 +229,9 @@
     <t>https://twitter.com/TheEagleTheatre</t>
   </si>
   <si>
+    <t>http://theeagletheatre.com/tickets/</t>
+  </si>
+  <si>
     <t>InterAct Theatre Company</t>
   </si>
   <si>
@@ -220,8 +241,7 @@
     <t>InterAct is a theatre for today's world, producing new and contemporary plays that explore the social, political, and cultural issues of our time. Founded in 1988, InterAct's aim is to educate and entertain its audiences by producing world-class, thought-provoking productions, and by using theatre as a tool to foster positive social change in the school, the workplace, and the community. Through its artistic and educational programs, InterAct seeks to make a significant contribution to the cultural life of Philadelphia and to the American theatre.</t>
   </si>
   <si>
-    <t>The Adrienne Theater, 
-2030 Sansom Street</t>
+    <t>2030 Sansom Street, Philadelphia</t>
   </si>
   <si>
     <t xml:space="preserve">215.568.8077
@@ -240,6 +260,9 @@
     <t>https://twitter.com/InterActThtrCo</t>
   </si>
   <si>
+    <t>http://interacttheatre.org/tickets/buy-tickets/</t>
+  </si>
+  <si>
     <t>People&amp;#039;s Light</t>
   </si>
   <si>
@@ -250,7 +273,7 @@
   </si>
   <si>
     <t>39 Conestoga Road, 
-Malvern, PA 19355</t>
+Malvern</t>
   </si>
   <si>
     <t xml:space="preserve">610.644.3500
@@ -269,6 +292,9 @@
     <t>https://twitter.com/peopleslight</t>
   </si>
   <si>
+    <t>http://peopleslight.org/buy-tickets</t>
+  </si>
+  <si>
     <t>Flashpoint Theatre Company</t>
   </si>
   <si>
@@ -278,8 +304,8 @@
     <t>Flashpoint Theatre Company produces socially provocative and emotionally resonant works of new and contemporary theatre in the Greater Philadelphia area, while giving voice to a diverse group of emerging artists.</t>
   </si>
   <si>
-    <t>1427 Spruce Street, Suite 1F, 
-Philadelphia, PA 19102</t>
+    <t>1427 Spruce Street, 
+Philadelphia</t>
   </si>
   <si>
     <t xml:space="preserve">267.997.3312
@@ -298,6 +324,9 @@
     <t>https://twitter.com/flashpointphila</t>
   </si>
   <si>
+    <t>http://flashpoint.ticketleap.com/</t>
+  </si>
+  <si>
     <t>Montgomery Theater</t>
   </si>
   <si>
@@ -308,7 +337,7 @@
   </si>
   <si>
     <t>124 N. Main Street, 
-Souderton, PA 18964</t>
+Souderton</t>
   </si>
   <si>
     <t xml:space="preserve">215.723.9945
@@ -327,6 +356,9 @@
     <t>https://twitter.com/MontgomTheater</t>
   </si>
   <si>
+    <t>http://boxoffice.printtixusa.com/montgomerytheater/eventcalendar</t>
+  </si>
+  <si>
     <t>Mazeppa Productions</t>
   </si>
   <si>
@@ -336,8 +368,7 @@
     <t>Mazeppa Productions is dedicated to the art of musical theatre. What you will see on our stage is simple – exciting, vibrant, and thought-provoking works of musical theatre. Some of our productions will be innovative productions of old favorites, some will be developmental productions of new works, and others will be productions meant to introduce the art form to a whole new generation. No matter what you see, we guarantee you will be exhilarated and challenged.</t>
   </si>
   <si>
-    <t>Christ Church Neighborhood House, 
-20 N. American Stree</t>
+    <t>20 N. American Street, Philadelphia</t>
   </si>
   <si>
     <t xml:space="preserve">267.559.9602
@@ -354,6 +385,36 @@
   </si>
   <si>
     <t>https://twitter.com/mazeppaprod</t>
+  </si>
+  <si>
+    <t>https://app.arts-people.com/index.php?ticketing=mazep</t>
+  </si>
+  <si>
+    <t>1427 Spruce Street, Philadelphia</t>
+  </si>
+  <si>
+    <t>Walnut Street Theater</t>
+  </si>
+  <si>
+    <t>http://www.walnutstreettheatre.org/</t>
+  </si>
+  <si>
+    <t>825 Walnut Street, Philadelphia</t>
+  </si>
+  <si>
+    <t>215 574-3550</t>
+  </si>
+  <si>
+    <t>https://www.walnutstreettheatre.org/contact.php</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/walnutstreettheatre</t>
+  </si>
+  <si>
+    <t>https://twitter.com/WalnutStTheatre</t>
+  </si>
+  <si>
+    <t>http://www.walnutstreettheatre.org/visit/box-office.php</t>
   </si>
 </sst>
 </file>
@@ -363,7 +424,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -380,9 +441,25 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="12"/>
       <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="11"/>
+      <name val="Book Antiqua"/>
     </font>
   </fonts>
   <fills count="2">
@@ -393,7 +470,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -416,27 +493,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -456,6 +597,8 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff0066cc"/>
+      <rgbColor rgb="ff333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1684,22 +1827,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="13.2" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="6.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.625" style="1" customWidth="1"/>
     <col min="5" max="5" width="6.625" style="1" customWidth="1"/>
     <col min="6" max="6" width="6.625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="6.625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="6.625" style="1" customWidth="1"/>
-    <col min="10" max="256" width="6.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.25" style="1" customWidth="1"/>
+    <col min="10" max="10" width="6.625" style="1" customWidth="1"/>
+    <col min="11" max="256" width="6.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
@@ -1709,7 +1853,7 @@
       <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" t="s" s="3">
         <v>2</v>
       </c>
       <c r="D1" t="s" s="2">
@@ -1730,388 +1874,628 @@
       <c r="I1" t="s" s="2">
         <v>8</v>
       </c>
+      <c r="J1" t="s" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" ht="26.65" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="C2" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="D2" t="s" s="5">
         <v>13</v>
       </c>
+      <c r="E2" t="s" s="5">
+        <v>14</v>
+      </c>
       <c r="F2" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J2" t="s" s="2">
+        <v>19</v>
       </c>
     </row>
     <row r="3" ht="26.65" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s" s="3">
         <v>21</v>
       </c>
-      <c r="E3" t="s" s="3">
+      <c r="C3" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="D3" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F3" s="6"/>
       <c r="G3" t="s" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="J3" t="s" s="2">
+        <v>28</v>
       </c>
     </row>
     <row r="4" ht="26.65" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s" s="3">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s" s="3">
         <v>30</v>
       </c>
+      <c r="C4" t="s" s="4">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s" s="5">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s" s="5">
+        <v>33</v>
+      </c>
       <c r="F4" t="s" s="2">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s" s="2">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="J4" t="s" s="2">
+        <v>38</v>
       </c>
     </row>
     <row r="5" ht="26.65" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="D5" t="s" s="3">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s" s="3">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C5" t="s" s="4">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s" s="5">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s" s="5">
+        <v>43</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="H5" t="s" s="2">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I5" t="s" s="2">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="J5" t="s" s="2">
+        <v>48</v>
       </c>
     </row>
     <row r="6" ht="26.65" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s" s="3">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s" s="3">
-        <v>13</v>
+        <v>50</v>
+      </c>
+      <c r="C6" t="s" s="4">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s" s="5">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s" s="5">
+        <v>53</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="H6" t="s" s="2">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="I6" t="s" s="2">
-        <v>17</v>
+        <v>57</v>
+      </c>
+      <c r="J6" t="s" s="2">
+        <v>58</v>
       </c>
     </row>
     <row r="7" ht="26.65" customHeight="1">
       <c r="A7" t="s" s="2">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="D7" t="s" s="3">
-        <v>47</v>
-      </c>
-      <c r="E7" t="s" s="3">
-        <v>48</v>
+        <v>60</v>
+      </c>
+      <c r="C7" t="s" s="4">
+        <v>61</v>
+      </c>
+      <c r="D7" t="s" s="5">
+        <v>62</v>
+      </c>
+      <c r="E7" t="s" s="5">
+        <v>63</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="H7" t="s" s="2">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="I7" t="s" s="2">
-        <v>52</v>
+        <v>67</v>
+      </c>
+      <c r="J7" t="s" s="2">
+        <v>68</v>
       </c>
     </row>
     <row r="8" ht="26.65" customHeight="1">
       <c r="A8" t="s" s="2">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="C8" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="D8" t="s" s="3">
-        <v>56</v>
-      </c>
-      <c r="E8" t="s" s="3">
-        <v>57</v>
+        <v>70</v>
+      </c>
+      <c r="C8" t="s" s="4">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s" s="5">
+        <v>72</v>
+      </c>
+      <c r="E8" t="s" s="5">
+        <v>73</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="H8" t="s" s="2">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="I8" t="s" s="2">
-        <v>61</v>
+        <v>77</v>
+      </c>
+      <c r="J8" t="s" s="2">
+        <v>78</v>
       </c>
     </row>
     <row r="9" ht="26.65" customHeight="1">
       <c r="A9" t="s" s="2">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="C9" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="D9" t="s" s="3">
-        <v>65</v>
-      </c>
-      <c r="E9" t="s" s="3">
-        <v>66</v>
+        <v>80</v>
+      </c>
+      <c r="C9" t="s" s="4">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s" s="5">
+        <v>82</v>
+      </c>
+      <c r="E9" t="s" s="5">
+        <v>83</v>
       </c>
       <c r="F9" t="s" s="2">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="H9" t="s" s="2">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="I9" t="s" s="2">
-        <v>70</v>
+        <v>87</v>
+      </c>
+      <c r="J9" t="s" s="2">
+        <v>88</v>
       </c>
     </row>
     <row r="10" ht="26.65" customHeight="1">
       <c r="A10" t="s" s="2">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="C10" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="D10" t="s" s="3">
-        <v>74</v>
-      </c>
-      <c r="E10" t="s" s="3">
-        <v>75</v>
+        <v>90</v>
+      </c>
+      <c r="C10" t="s" s="4">
+        <v>91</v>
+      </c>
+      <c r="D10" t="s" s="5">
+        <v>92</v>
+      </c>
+      <c r="E10" t="s" s="5">
+        <v>93</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="I10" t="s" s="2">
-        <v>79</v>
+        <v>97</v>
+      </c>
+      <c r="J10" t="s" s="2">
+        <v>98</v>
       </c>
     </row>
     <row r="11" ht="26.65" customHeight="1">
       <c r="A11" t="s" s="2">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="C11" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="D11" t="s" s="3">
-        <v>83</v>
-      </c>
-      <c r="E11" t="s" s="3">
-        <v>84</v>
+        <v>100</v>
+      </c>
+      <c r="C11" t="s" s="4">
+        <v>101</v>
+      </c>
+      <c r="D11" t="s" s="5">
+        <v>102</v>
+      </c>
+      <c r="E11" t="s" s="5">
+        <v>103</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>88</v>
+        <v>107</v>
+      </c>
+      <c r="J11" t="s" s="2">
+        <v>108</v>
       </c>
     </row>
     <row r="12" ht="26.65" customHeight="1">
       <c r="A12" t="s" s="2">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>90</v>
-      </c>
-      <c r="C12" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="D12" t="s" s="3">
-        <v>92</v>
-      </c>
-      <c r="E12" t="s" s="3">
-        <v>93</v>
+        <v>110</v>
+      </c>
+      <c r="C12" t="s" s="7">
+        <v>111</v>
+      </c>
+      <c r="D12" t="s" s="5">
+        <v>112</v>
+      </c>
+      <c r="E12" t="s" s="5">
+        <v>113</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>97</v>
+        <v>117</v>
+      </c>
+      <c r="J12" t="s" s="2">
+        <v>118</v>
       </c>
     </row>
     <row r="13" ht="26.65" customHeight="1">
       <c r="A13" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" t="s" s="5">
+        <v>119</v>
+      </c>
+      <c r="E13" t="s" s="5">
+        <v>93</v>
+      </c>
+      <c r="F13" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="G13" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="H13" t="s" s="2">
+        <v>96</v>
+      </c>
+      <c r="I13" t="s" s="2">
+        <v>97</v>
+      </c>
+      <c r="J13" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="B13" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="C13" t="s" s="2">
-        <v>100</v>
-      </c>
-      <c r="D13" t="s" s="3">
-        <v>101</v>
-      </c>
-      <c r="E13" t="s" s="3">
-        <v>102</v>
-      </c>
-      <c r="F13" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="G13" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="H13" t="s" s="2">
-        <v>105</v>
-      </c>
-      <c r="I13" t="s" s="2">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" ht="26.65" customHeight="1">
+    </row>
+    <row r="14" ht="16" customHeight="1">
       <c r="A14" t="s" s="2">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="C14" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="D14" t="s" s="3">
-        <v>74</v>
-      </c>
-      <c r="E14" t="s" s="3">
-        <v>75</v>
+        <v>121</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="E14" t="s" s="2">
+        <v>123</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>77</v>
+        <v>121</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>78</v>
+        <v>125</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>79</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="J14" t="s" s="2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" ht="17" customHeight="1">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddHeader>
-    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;10&amp;K000000zingvenues.xls</oddFooter>
+    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;10&amp;K000000Copy of zingvenues.xls</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="13.2" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="6.625" style="12" customWidth="1"/>
+    <col min="2" max="2" width="6.625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="6.625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="6.625" style="12" customWidth="1"/>
+    <col min="6" max="256" width="6.625" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.65" customHeight="1">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" ht="15.65" customHeight="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" ht="15.65" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" ht="15.65" customHeight="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" ht="15.65" customHeight="1">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" ht="15.65" customHeight="1">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" ht="15.65" customHeight="1">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" ht="15.65" customHeight="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" ht="15.65" customHeight="1">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" ht="15.65" customHeight="1">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="13.2" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="6.625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="6.625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="6.625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="6.625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="6.625" style="13" customWidth="1"/>
+    <col min="6" max="256" width="6.625" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15.65" customHeight="1">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" ht="15.65" customHeight="1">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" ht="15.65" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" ht="15.65" customHeight="1">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" ht="15.65" customHeight="1">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" ht="15.65" customHeight="1">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" ht="15.65" customHeight="1">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" ht="15.65" customHeight="1">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" ht="15.65" customHeight="1">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" ht="15.65" customHeight="1">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>